<commit_message>
feat: Implement core LLM processing and task distribution logic with associated interaction logs and static report.
</commit_message>
<xml_diff>
--- a/src/static/Reporte_2026_ENERO.xlsx
+++ b/src/static/Reporte_2026_ENERO.xlsx
@@ -688,7 +688,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Análisis del sistema de OCR</t>
+          <t>Planificación de la implementación de FastAPI</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E4" s="12" t="inlineStr">
         <is>
@@ -708,7 +708,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Implementación del backend FastAPI</t>
+          <t>Sincronización diaria con el equipo y actualización de estado</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -717,9 +717,9 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
-      </c>
-      <c r="H5" s="12" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="E5" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -728,7 +728,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Configuración inicial del proyecto</t>
+          <t>Revisión de documentación y notas técnicas</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -737,9 +737,9 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
-      </c>
-      <c r="I6" s="12" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="E6" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -748,7 +748,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Optimización de código y reducción de deuda técnica</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -757,9 +757,9 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
-      </c>
-      <c r="J7" s="12" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="E7" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -768,7 +768,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Discusión técnica interna y planificación</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -777,9 +777,9 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>8</v>
-      </c>
-      <c r="K8" s="12" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="E8" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -788,7 +788,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Implementación de FastAPI backend para OCR y procesamiento de documentos</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -797,9 +797,9 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
-      </c>
-      <c r="L9" s="12" t="inlineStr">
+        <v>2.5</v>
+      </c>
+      <c r="H9" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -808,7 +808,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Sincronización diaria con el equipo y actualización de estado</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -817,9 +817,9 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8</v>
-      </c>
-      <c r="P10" s="12" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="H10" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -828,7 +828,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Revisión de documentación y notas técnicas</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -837,9 +837,9 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8</v>
-      </c>
-      <c r="Q11" s="12" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="H11" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -848,7 +848,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Optimización de código y reducción de deuda técnica</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -857,9 +857,9 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8</v>
-      </c>
-      <c r="R12" s="12" t="inlineStr">
+        <v>1.5</v>
+      </c>
+      <c r="H12" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -868,7 +868,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Configuración del servidor backend con FastAPI</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -877,9 +877,9 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>8</v>
-      </c>
-      <c r="S13" s="12" t="inlineStr">
+        <v>0.5</v>
+      </c>
+      <c r="I13" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -888,7 +888,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Sincronización diaria con el equipo y actualización de estado</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -897,9 +897,9 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>8</v>
-      </c>
-      <c r="V14" s="12" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="I14" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -908,7 +908,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Revisión de documentación y notas técnicas</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -917,9 +917,9 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8</v>
-      </c>
-      <c r="W15" s="12" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="I15" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -928,7 +928,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Optimización de código y reducción de deuda técnica</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -937,9 +937,9 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>8</v>
-      </c>
-      <c r="X16" s="12" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="I16" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -948,7 +948,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Discusión técnica interna y planificación</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -957,9 +957,9 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>8</v>
-      </c>
-      <c r="Y17" s="12" t="inlineStr">
+        <v>1.5</v>
+      </c>
+      <c r="I17" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Creación de ejemplo de estructura de declaración financiera con data</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -977,9 +977,9 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>8</v>
-      </c>
-      <c r="Z18" s="12" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="J18" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -988,7 +988,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Sincronización diaria con el equipo y actualización de estado</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -997,9 +997,9 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>8</v>
-      </c>
-      <c r="AC19" s="12" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="J19" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1008,7 +1008,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Revisión de documentación y notas técnicas</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1017,9 +1017,9 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>8</v>
-      </c>
-      <c r="AD20" s="12" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="J20" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1028,7 +1028,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Optimización de código y reducción de deuda técnica</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1037,9 +1037,9 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8</v>
-      </c>
-      <c r="AE21" s="12" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="J21" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1048,7 +1048,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>General review and maintenance of systems</t>
+          <t>Discusión técnica interna y planificación</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1057,9 +1057,9 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>8</v>
-      </c>
-      <c r="AF22" s="12" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="J22" s="12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1068,91 +1068,1383 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>Implementación de autenticación en el backend</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K23" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Sincronización diaria con el equipo y actualización de estado</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>2</v>
+      </c>
+      <c r="K24" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Revisión de documentación y notas técnicas</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>2</v>
+      </c>
+      <c r="K25" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Optimización de código y reducción de deuda técnica</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K26" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Definición de ruta y endpoints en FastAPI</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L27" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Sincronización diaria con el equipo y actualización de estado</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>2</v>
+      </c>
+      <c r="L28" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Revisión de documentación y notas técnicas</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>2</v>
+      </c>
+      <c r="L29" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Optimización de código y reducción de deuda técnica</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>2</v>
+      </c>
+      <c r="L30" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Discusión técnica interna y planificación</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="L31" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Conexión con bases de datos y almacenamiento de datos</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="P32" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Sincronización diaria con el equipo y actualización de estado</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>2</v>
+      </c>
+      <c r="P33" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Revisión de documentación y notas técnicas</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>2</v>
+      </c>
+      <c r="P34" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Optimización de código y reducción de deuda técnica</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>2</v>
+      </c>
+      <c r="P35" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Discusión técnica interna y planificación</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="P36" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Implementación de clasificación de transacciones</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q37" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Sincronización diaria con el equipo y actualización de estado</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q38" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Revisión de documentación y notas técnicas</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q39" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Optimización de código y reducción de deuda técnica</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q40" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Configuración del entorno de desarrollo para FastAPI</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R41" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Sincronización diaria con el equipo y actualización de estado</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>2</v>
+      </c>
+      <c r="R42" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Revisión de documentación y notas técnicas</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>2</v>
+      </c>
+      <c r="R43" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Optimización de código y reducción de deuda técnica</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>2</v>
+      </c>
+      <c r="R44" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Discusión técnica interna y planificación</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="R45" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Realización de pruebas unitarias y de integración</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>1</v>
+      </c>
+      <c r="S46" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Sincronización diaria con el equipo y actualización de estado</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>2</v>
+      </c>
+      <c r="S47" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Revisión de documentación y notas técnicas</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>2</v>
+      </c>
+      <c r="S48" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Optimización de código y reducción de deuda técnica</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>2</v>
+      </c>
+      <c r="S49" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Discusión técnica interna y planificación</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
+      <c r="S50" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Creación de documentación de API y herramientas adicionales</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>2</v>
+      </c>
+      <c r="V51" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Sincronización diaria con el equipo y actualización de estado</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>2</v>
+      </c>
+      <c r="V52" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Revisión de documentación y notas técnicas</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>2</v>
+      </c>
+      <c r="V53" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Optimización de código y reducción de deuda técnica</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>2</v>
+      </c>
+      <c r="V54" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Implementación de seguridad y autenticación en el backend</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>3</v>
+      </c>
+      <c r="W55" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Sincronización diaria con el equipo y actualización de estado</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>2</v>
+      </c>
+      <c r="W56" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Revisión de documentación y notas técnicas</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>2</v>
+      </c>
+      <c r="W57" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Optimización de código y reducción de deuda técnica</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>1</v>
+      </c>
+      <c r="W58" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Finalización del desarrollo y ajuste de pruebas</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="X59" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Sincronización diaria con el equipo y actualización de estado</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>2</v>
+      </c>
+      <c r="X60" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Revisión de documentación y notas técnicas</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>2</v>
+      </c>
+      <c r="X61" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Optimización de código y reducción de deuda técnica</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>2</v>
+      </c>
+      <c r="X62" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Discusión técnica interna y planificación</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="X63" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Desplegar la aplicación al entorno de producción</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y64" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Sincronización diaria con el equipo y actualización de estado</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y65" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Revisión de documentación y notas técnicas</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y66" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Optimización de código y reducción de deuda técnica</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y67" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
           <t>General review and maintenance of systems</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Synaptica</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>8</v>
-      </c>
-      <c r="AG23" s="12" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z68" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Code optimization and technical debt reduction</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z69" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Documentation updates and process review</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z70" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Security patches and dependency updates</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z71" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>General review and maintenance of systems</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC72" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Code optimization and technical debt reduction</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC73" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Documentation updates and process review</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC74" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Security patches and dependency updates</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC75" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>General review and maintenance of systems</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD76" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Code optimization and technical debt reduction</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD77" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Documentation updates and process review</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD78" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Security patches and dependency updates</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD79" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>General review and maintenance of systems</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE80" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Code optimization and technical debt reduction</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE81" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Documentation updates and process review</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE82" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Security patches and dependency updates</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE83" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>General review and maintenance of systems</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF84" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Code optimization and technical debt reduction</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF85" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Documentation updates and process review</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF86" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Security patches and dependency updates</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF87" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>General review and maintenance of systems</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG88" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Code optimization and technical debt reduction</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG89" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Documentation updates and process review</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG90" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Security patches and dependency updates</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Synaptica</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG91" s="12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
     <row r="92"/>
     <row r="93"/>
     <row r="94"/>

</xml_diff>